<commit_message>
Packing subjects with times works but iterating is still not working correctly => Error in packData function
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Programming\Python\Excel_Parser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Python_Programs\Excel_Parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5642011-1F9C-49A7-9B61-9188F5887247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADCB17B-7396-4F8F-AB3A-63D3C3EEB949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="2280" windowWidth="15255" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatik" sheetId="1" r:id="rId1"/>
@@ -997,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1364,6 +1364,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1600,7 +1603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G42" sqref="G42"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1710,7 @@
       <c r="B5" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="132" t="s">
         <v>120</v>
       </c>
       <c r="D5" s="73" t="s">

</xml_diff>